<commit_message>
Update SNSP limits according to historic data current projections
Historic data:
- https://www.eirgridgroup.com/newsroom/record-renewable-energy-o/index.xml
- https://www.eirgridgroup.com/how-the-grid-works/ds3-programme/
- https://www.eirgridgroup.com/newsroom/electricity-grid-to-run-o/index.xml

Projections (until 2030):
- https://www.eirgridgroup.com/site-files/library/EirGrid/Shaping_Our_Electricity_Future_Roadmap.pdf
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_PWR_SNSP.xlsx
+++ b/SuppXLS/Scen_B_PWR_SNSP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A05B87C-615E-421D-A9BC-50DFC14467EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620C1DDA-E78F-4EB2-BEF0-62F5D1ECAE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5565" yWindow="-18120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5640" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="100">
   <si>
     <t>UC_N</t>
   </si>
@@ -465,7 +465,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -785,7 +785,7 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -797,6 +797,8 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -806,8 +808,6 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{D98056AC-E05F-4C3F-AD8B-5B1524962E09}"/>
@@ -1967,12 +1967,12 @@
       <c r="Z15" s="24"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
       <c r="E16" s="26"/>
       <c r="F16" s="26"/>
       <c r="G16" s="27"/>
@@ -2056,11 +2056,11 @@
       <c r="A19" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
       <c r="G19" s="33"/>
@@ -2088,11 +2088,11 @@
       <c r="A20" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
       <c r="E20" s="32"/>
       <c r="F20" s="32"/>
       <c r="G20" s="33"/>
@@ -2180,11 +2180,11 @@
       <c r="A23" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
       <c r="G23" s="24"/>
@@ -2268,11 +2268,11 @@
       <c r="A26" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
       <c r="E26" s="24"/>
       <c r="F26" s="24"/>
       <c r="G26" s="24"/>
@@ -2388,11 +2388,11 @@
       <c r="A30" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
       <c r="E30" s="36"/>
       <c r="F30" s="36"/>
       <c r="G30" s="24"/>
@@ -2420,11 +2420,11 @@
       <c r="A31" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
       <c r="E31" s="36"/>
       <c r="F31" s="36"/>
       <c r="G31" s="24"/>
@@ -5143,10 +5143,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5266,25 +5266,25 @@
       <c r="D8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="13" t="s">
+      <c r="E8" s="16"/>
+      <c r="F8" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11">
-        <v>2020</v>
-      </c>
-      <c r="K8" s="11" t="s">
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16">
+        <v>2018</v>
+      </c>
+      <c r="K8" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="L8" s="42">
-        <v>-0.5</v>
-      </c>
-      <c r="M8" s="43">
+      <c r="L8" s="39">
+        <v>-0.65</v>
+      </c>
+      <c r="M8" s="40">
         <v>0</v>
       </c>
       <c r="N8" s="12" t="s">
@@ -5301,20 +5301,21 @@
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11">
-        <v>2020</v>
-      </c>
-      <c r="K9" s="11"/>
-      <c r="L9" s="42">
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16">
+        <f>J8</f>
+        <v>2018</v>
+      </c>
+      <c r="K9" s="16"/>
+      <c r="L9" s="39">
         <f>1+L8</f>
-        <v>0.5</v>
-      </c>
-      <c r="M9" s="43"/>
+        <v>0.35</v>
+      </c>
+      <c r="M9" s="40"/>
       <c r="N9" s="11"/>
       <c r="O9" s="3"/>
     </row>
@@ -5325,25 +5326,25 @@
       <c r="D10" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="14" t="s">
+      <c r="E10" s="11"/>
+      <c r="F10" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3">
-        <v>2025</v>
-      </c>
-      <c r="K10" s="3" t="s">
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11">
+        <v>2020</v>
+      </c>
+      <c r="K10" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="L10" s="42">
-        <v>-0.7</v>
-      </c>
-      <c r="M10" s="43">
+      <c r="L10" s="39">
+        <v>-0.65</v>
+      </c>
+      <c r="M10" s="40">
         <v>0</v>
       </c>
     </row>
@@ -5356,18 +5357,21 @@
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="J11" s="3">
-        <v>2025</v>
-      </c>
-      <c r="L11" s="42">
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="16">
+        <f>J10</f>
+        <v>2020</v>
+      </c>
+      <c r="K11" s="11"/>
+      <c r="L11" s="39">
         <f>1+L10</f>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="M11" s="43"/>
+        <v>0.35</v>
+      </c>
+      <c r="M11" s="40"/>
     </row>
     <row r="12" spans="1:15">
       <c r="C12" s="14" t="s">
@@ -5384,16 +5388,17 @@
         <v>79</v>
       </c>
       <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
       <c r="J12" s="3">
-        <v>2030</v>
-      </c>
-      <c r="K12" t="s">
+        <v>2021</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="L12" s="42">
-        <v>-1</v>
-      </c>
-      <c r="M12" s="43">
+      <c r="L12" s="39">
+        <v>-0.7</v>
+      </c>
+      <c r="M12" s="40">
         <v>0</v>
       </c>
     </row>
@@ -5410,14 +5415,15 @@
         <v>79</v>
       </c>
       <c r="H13" s="3"/>
-      <c r="J13" s="3">
-        <v>2030</v>
-      </c>
-      <c r="L13" s="42">
+      <c r="J13" s="16">
+        <f>J12</f>
+        <v>2021</v>
+      </c>
+      <c r="L13" s="39">
         <f>1+L12</f>
-        <v>0</v>
-      </c>
-      <c r="M13" s="43"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="M13" s="40"/>
     </row>
     <row r="14" spans="1:15">
       <c r="C14" s="14" t="s">
@@ -5435,15 +5441,15 @@
       </c>
       <c r="H14" s="3"/>
       <c r="J14" s="3">
-        <v>2050</v>
+        <v>2022</v>
       </c>
       <c r="K14" t="s">
         <v>98</v>
       </c>
-      <c r="L14" s="42">
-        <v>-1</v>
-      </c>
-      <c r="M14" s="43">
+      <c r="L14" s="39">
+        <v>-0.75</v>
+      </c>
+      <c r="M14" s="40">
         <v>0</v>
       </c>
     </row>
@@ -5459,23 +5465,323 @@
       <c r="G15" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="J15" s="3">
-        <v>2050</v>
-      </c>
-      <c r="L15" s="42">
+      <c r="H15" s="3"/>
+      <c r="J15" s="16">
+        <f>J14</f>
+        <v>2022</v>
+      </c>
+      <c r="L15" s="39">
         <f>1+L14</f>
+        <v>0.25</v>
+      </c>
+      <c r="M15" s="40"/>
+    </row>
+    <row r="16" spans="1:15" s="16" customFormat="1">
+      <c r="C16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="J16" s="3">
+        <v>2024</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="L16" s="39">
+        <v>-0.75</v>
+      </c>
+      <c r="M16" s="40">
         <v>0</v>
       </c>
-      <c r="M15" s="43"/>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="J16" s="3">
+    </row>
+    <row r="17" spans="3:13" s="16" customFormat="1">
+      <c r="C17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="J17" s="16">
+        <f>J16</f>
+        <v>2024</v>
+      </c>
+      <c r="L17" s="39">
+        <f>1+L16</f>
+        <v>0.25</v>
+      </c>
+      <c r="M17" s="40"/>
+    </row>
+    <row r="18" spans="3:13" s="16" customFormat="1">
+      <c r="C18" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="J18" s="3">
+        <v>2025</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="L18" s="39">
+        <v>-0.85</v>
+      </c>
+      <c r="M18" s="40">
         <v>0</v>
       </c>
-      <c r="K16" t="s">
+    </row>
+    <row r="19" spans="3:13" s="16" customFormat="1">
+      <c r="C19" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="J19" s="16">
+        <f>J18</f>
+        <v>2025</v>
+      </c>
+      <c r="L19" s="39">
+        <f>1+L18</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="M19" s="40"/>
+    </row>
+    <row r="20" spans="3:13" s="16" customFormat="1">
+      <c r="C20" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="J20" s="3">
+        <v>2029</v>
+      </c>
+      <c r="K20" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="M16">
+      <c r="L20" s="39">
+        <v>-0.85</v>
+      </c>
+      <c r="M20" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" s="16" customFormat="1">
+      <c r="C21" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="J21" s="16">
+        <f>J20</f>
+        <v>2029</v>
+      </c>
+      <c r="L21" s="39">
+        <f>1+L20</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="M21" s="40"/>
+    </row>
+    <row r="22" spans="3:13">
+      <c r="C22" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="16"/>
+      <c r="F22" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="J22" s="3">
+        <v>2030</v>
+      </c>
+      <c r="K22" t="s">
+        <v>98</v>
+      </c>
+      <c r="L22" s="39">
+        <v>-0.95</v>
+      </c>
+      <c r="M22" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13">
+      <c r="C23" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="J23" s="16">
+        <f>J22</f>
+        <v>2030</v>
+      </c>
+      <c r="L23" s="39">
+        <f>1+L22</f>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="M23" s="40"/>
+    </row>
+    <row r="24" spans="3:13" s="16" customFormat="1">
+      <c r="C24" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H24" s="3"/>
+      <c r="J24" s="3">
+        <v>2034</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="L24" s="39">
+        <v>-0.95</v>
+      </c>
+      <c r="M24" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13" s="16" customFormat="1">
+      <c r="C25" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="J25" s="16">
+        <f>J24</f>
+        <v>2034</v>
+      </c>
+      <c r="L25" s="39">
+        <f>1+L24</f>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="M25" s="40"/>
+    </row>
+    <row r="26" spans="3:13" s="16" customFormat="1">
+      <c r="C26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H26" s="3"/>
+      <c r="J26" s="3">
+        <v>2035</v>
+      </c>
+      <c r="K26" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="L26" s="39">
+        <v>-1</v>
+      </c>
+      <c r="M26" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" s="16" customFormat="1">
+      <c r="C27" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="J27" s="16">
+        <f>J26</f>
+        <v>2035</v>
+      </c>
+      <c r="L27" s="39">
+        <f>1+L26</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="40"/>
+    </row>
+    <row r="28" spans="3:13">
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+      <c r="K28" t="s">
+        <v>98</v>
+      </c>
+      <c r="M28">
         <v>5</v>
       </c>
     </row>

</xml_diff>